<commit_message>
added time estimate on product backlog
</commit_message>
<xml_diff>
--- a/docs/cs1/task10/scrum_v02.xlsx
+++ b/docs/cs1/task10/scrum_v02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" state="visible" r:id="rId2"/>
@@ -97,22 +97,22 @@
     <t xml:space="preserve">The user adds an appointment </t>
   </si>
   <si>
+    <t xml:space="preserve">medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waiting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User selects appointment to get displayed</t>
+  </si>
+  <si>
     <t xml:space="preserve">high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View appointment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User selects appointment to get displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medium</t>
   </si>
   <si>
     <t xml:space="preserve">Complete appointment</t>
@@ -492,8 +492,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -548,6 +548,9 @@
       <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E2" s="2" t="n">
+        <v>10</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
@@ -568,6 +571,9 @@
       <c r="D3" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>20</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
@@ -588,6 +594,9 @@
       <c r="D4" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
@@ -606,7 +615,10 @@
         <v>34</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
@@ -626,7 +638,10 @@
         <v>36</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>25</v>
@@ -653,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -792,7 +807,7 @@
         <v>50</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>7</v>
@@ -821,7 +836,7 @@
         <v>49</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>7</v>
@@ -850,7 +865,7 @@
         <v>54</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>7</v>
@@ -879,7 +894,7 @@
         <v>53</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
update by scrum daily 10.05.2017
</commit_message>
<xml_diff>
--- a/docs/cs1/task10/scrum_v02.xlsx
+++ b/docs/cs1/task10/scrum_v02.xlsx
@@ -913,7 +913,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1031,7 +1031,7 @@
         <v>7</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L4" t="s">
         <v>26</v>
@@ -1063,7 +1063,7 @@
         <v>7</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" t="s">
         <v>26</v>
@@ -1127,7 +1127,7 @@
         <v>7</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L7" t="s">
         <v>26</v>
@@ -1159,7 +1159,7 @@
         <v>7</v>
       </c>
       <c r="K8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L8" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updates in srcum backlog
</commit_message>
<xml_diff>
--- a/docs/cs1/task10/scrum_v02.xlsx
+++ b/docs/cs1/task10/scrum_v02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" state="visible" r:id="rId2"/>
@@ -440,13 +440,13 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -523,16 +523,16 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.51417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,21 +695,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.7397959183674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.51417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.51417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.51417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5384615384615"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,10 +1046,10 @@
         <v>50</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>14</v>
@@ -1077,6 +1077,9 @@
       <c r="I12" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="J12" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1100,6 +1103,9 @@
       <c r="I13" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="J13" s="0" t="n">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1115,13 +1121,16 @@
         <v>50</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>14</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,6 +1155,9 @@
       <c r="I15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1168,6 +1180,42 @@
       </c>
       <c r="I16" s="0" t="n">
         <v>14</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1188,13 +1236,13 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Scrum sprint 2 fertig gestellt
</commit_message>
<xml_diff>
--- a/docs/cs1/task10/scrum_v02.xlsx
+++ b/docs/cs1/task10/scrum_v02.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -249,6 +249,36 @@
   </si>
   <si>
     <t>Moved</t>
+  </si>
+  <si>
+    <t>Design verbessern</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Navigation von Appointment zu Patient View</t>
+  </si>
+  <si>
+    <t>Abschlussdialog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>Unit Tests</t>
+  </si>
+  <si>
+    <t>Testdaten generiern</t>
+  </si>
+  <si>
+    <t>Design responsive machen</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -902,14 +932,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1043,7 +1074,7 @@
         <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I5">
         <v>7</v>
@@ -1078,7 +1109,7 @@
         <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I6">
         <v>7</v>
@@ -1113,7 +1144,7 @@
         <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I7">
         <v>7</v>
@@ -1183,7 +1214,7 @@
         <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I9">
         <v>7</v>
@@ -1218,7 +1249,7 @@
         <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I10">
         <v>7</v>
@@ -1265,7 +1296,7 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1358,7 +1389,7 @@
         <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I14">
         <v>14</v>
@@ -1367,10 +1398,10 @@
         <v>14</v>
       </c>
       <c r="K14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L14" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1405,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="L15" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1443,37 +1474,284 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>2.9</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>3.1</v>
       </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>14</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3.2</v>
+      </c>
       <c r="B19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>14</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3.3</v>
+      </c>
       <c r="B20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>7</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3.4</v>
+      </c>
       <c r="B21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21">
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3.5</v>
+      </c>
       <c r="B22">
         <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3.6</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+      <c r="J23">
+        <v>7</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3.7</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scrum sprint 3 aktuallisiert
</commit_message>
<xml_diff>
--- a/docs/cs1/task10/scrum_v02.xlsx
+++ b/docs/cs1/task10/scrum_v02.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>medium</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>View appointment</t>
   </si>
   <si>
@@ -129,12 +126,6 @@
   </si>
   <si>
     <t>low</t>
-  </si>
-  <si>
-    <t>0h</t>
-  </si>
-  <si>
-    <t>waiting</t>
   </si>
   <si>
     <t>manage patient data</t>
@@ -725,13 +716,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -801,12 +794,15 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -835,7 +831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -849,13 +845,16 @@
         <v>24</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="F2" s="2">
+        <v>26</v>
       </c>
       <c r="G2" s="2">
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -863,25 +862,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
       <c r="E3">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F3">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2">
         <v>40</v>
       </c>
-      <c r="G3" s="2">
-        <v>31</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -889,22 +888,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
       <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2">
+        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -912,22 +914,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="F5">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2">
+        <v>46</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -935,22 +940,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="F6">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2">
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -963,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,7 +988,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -989,13 +997,13 @@
         <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>17</v>
@@ -1021,21 +1029,21 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
       <c r="I3">
         <v>7</v>
       </c>
@@ -1046,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1057,21 +1065,21 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
       <c r="I4">
         <v>7</v>
       </c>
@@ -1082,7 +1090,7 @@
         <v>7</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1093,19 +1101,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>49</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" t="s">
-        <v>53</v>
       </c>
       <c r="I5">
         <v>7</v>
@@ -1117,7 +1125,7 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1128,19 +1136,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
       </c>
       <c r="I6">
         <v>7</v>
@@ -1152,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1163,20 +1171,20 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
         <v>50</v>
       </c>
-      <c r="F7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
       <c r="I7">
         <v>7</v>
       </c>
@@ -1187,7 +1195,7 @@
         <v>7</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1198,20 +1206,20 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
         <v>43</v>
       </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
       <c r="I8">
         <v>7</v>
       </c>
@@ -1222,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1233,20 +1241,20 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" t="s">
-        <v>53</v>
-      </c>
       <c r="I9">
         <v>7</v>
       </c>
@@ -1257,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1268,19 +1276,19 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
         <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" t="s">
-        <v>53</v>
       </c>
       <c r="I10">
         <v>7</v>
@@ -1292,7 +1300,7 @@
         <v>10</v>
       </c>
       <c r="L10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1303,19 +1311,19 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I11">
         <v>10</v>
@@ -1327,7 +1335,7 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1338,19 +1346,19 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I12">
         <v>4</v>
@@ -1362,7 +1370,7 @@
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1373,19 +1381,19 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I13">
         <v>14</v>
@@ -1397,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="L13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1408,19 +1416,19 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
         <v>50</v>
-      </c>
-      <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" t="s">
-        <v>53</v>
       </c>
       <c r="I14">
         <v>14</v>
@@ -1432,7 +1440,7 @@
         <v>7</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1443,19 +1451,19 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I15">
         <v>14</v>
@@ -1467,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1478,19 +1486,19 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
         <v>43</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>46</v>
       </c>
       <c r="I16">
         <v>14</v>
@@ -1502,7 +1510,7 @@
         <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1513,19 +1521,19 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I17">
         <v>7</v>
@@ -1537,7 +1545,7 @@
         <v>7</v>
       </c>
       <c r="L17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1548,19 +1556,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I18">
         <v>5</v>
@@ -1572,7 +1580,7 @@
         <v>5</v>
       </c>
       <c r="L18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1583,19 +1591,19 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1607,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1618,19 +1626,19 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I20">
         <v>10</v>
@@ -1642,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="L20" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1653,19 +1661,19 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" t="s">
         <v>50</v>
-      </c>
-      <c r="F21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" t="s">
-        <v>53</v>
       </c>
       <c r="I21">
         <v>14</v>
@@ -1677,7 +1685,7 @@
         <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1688,19 +1696,19 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I22">
         <v>7</v>
@@ -1709,10 +1717,10 @@
         <v>7</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L22" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1723,19 +1731,19 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I23">
         <v>7</v>
@@ -1744,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L23" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1758,19 +1766,19 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I24">
         <v>7</v>
@@ -1779,10 +1787,10 @@
         <v>7</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1793,19 +1801,19 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I25">
         <v>3</v>
@@ -1814,10 +1822,10 @@
         <v>3</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L25" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1828,19 +1836,19 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I26">
         <v>3</v>
@@ -1849,10 +1857,10 @@
         <v>3</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L26" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1863,19 +1871,19 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I27">
         <v>14</v>
@@ -1884,10 +1892,10 @@
         <v>14</v>
       </c>
       <c r="K27">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L27" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1901,26 +1909,30 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>